<commit_message>
added numberformatinfo properties but still inactive
</commit_message>
<xml_diff>
--- a/LocaleInformationConstants.xlsx
+++ b/LocaleInformationConstants.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1753" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="396">
   <si>
     <t>LOCALE_ALL</t>
   </si>
@@ -1432,6 +1432,12 @@
   </si>
   <si>
     <t>L"!x-sys-default-locale"</t>
+  </si>
+  <si>
+    <t>LOCALE_SRELATIVELONGDATE</t>
+  </si>
+  <si>
+    <t>&amp;H7C</t>
   </si>
 </sst>
 </file>
@@ -1809,10 +1815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E211"/>
+  <dimension ref="A1:E213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="A213" sqref="A213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4634,6 +4640,14 @@
       <c r="E211">
         <f t="shared" si="3"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>394</v>
+      </c>
+      <c r="B213" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -4750,9 +4764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G211"/>
   <sheetViews>
-    <sheetView topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="F200" sqref="F200:G207"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8870,9 +8882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8938,9 +8948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>